<commit_message>
incorporating hybrid model, new gas forecasts
</commit_message>
<xml_diff>
--- a/data/US_GasPrice_2020-2050.xlsx
+++ b/data/US_GasPrice_2020-2050.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\UT_Grad\EDP_LAW379M\EnviroDev_Policy\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\UT_Grad\EDP_LAW379M\EnergyDevelopment_Policy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4612076D-A5C1-45C5-9101-75177526156E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63159049-D653-428E-8B16-A3F42B8F6ECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-4650" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -59,7 +70,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +201,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -492,7 +510,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -535,12 +553,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -578,6 +597,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="42" xr:uid="{AACBD050-A29A-43AB-A7B0-03ED4B1BEA17}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -894,13 +914,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -939,1240 +971,750 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="B2">
-        <v>3.5362040000000001</v>
+        <v>1.9503086606661479</v>
       </c>
       <c r="C2">
-        <v>3.5362040000000001</v>
+        <v>2.0478240936994556</v>
       </c>
       <c r="D2">
-        <v>3.536206</v>
+        <v>5.1183149999999999</v>
       </c>
       <c r="E2">
-        <v>3.5361899999999999</v>
+        <v>5.1889880000000002</v>
       </c>
       <c r="F2">
-        <v>3.5362279999999999</v>
+        <v>4.8038080000000001</v>
       </c>
       <c r="G2">
-        <v>3.536187</v>
+        <v>4.6971639999999999</v>
       </c>
       <c r="H2">
-        <v>3.5361850000000001</v>
+        <v>6.6139939999999999</v>
       </c>
       <c r="I2">
-        <v>3.536171</v>
+        <v>5.1673260000000001</v>
       </c>
       <c r="J2">
-        <v>3.536187</v>
+        <v>5.1110220000000002</v>
       </c>
       <c r="K2">
-        <v>3.5361859999999998</v>
+        <v>5.1855979999999997</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="B3">
-        <v>4.0974329999999997</v>
+        <v>2.879269540309906</v>
       </c>
       <c r="C3">
-        <v>4.0973610000000003</v>
+        <v>3.0232330173254014</v>
       </c>
       <c r="D3">
-        <v>4.0974760000000003</v>
+        <v>5.2508660000000003</v>
       </c>
       <c r="E3">
-        <v>4.0984569999999998</v>
+        <v>5.2204249999999996</v>
       </c>
       <c r="F3">
-        <v>4.0974110000000001</v>
+        <v>4.9484219999999999</v>
       </c>
       <c r="G3">
-        <v>4.0966940000000003</v>
+        <v>4.5277120000000002</v>
       </c>
       <c r="H3">
-        <v>4.0974300000000001</v>
+        <v>7.0335140000000003</v>
       </c>
       <c r="I3">
-        <v>4.0973730000000002</v>
+        <v>5.2257680000000004</v>
       </c>
       <c r="J3">
-        <v>4.0973139999999999</v>
+        <v>5.1857009999999999</v>
       </c>
       <c r="K3">
-        <v>4.0975149999999996</v>
+        <v>5.3002320000000003</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2018</v>
+        <v>2022</v>
       </c>
       <c r="B4">
-        <v>4.2567009999999996</v>
+        <v>2.8612766861915588</v>
       </c>
       <c r="C4">
-        <v>4.2399459999999998</v>
+        <v>3.0043405205011369</v>
       </c>
       <c r="D4">
-        <v>4.267849</v>
+        <v>5.4649460000000003</v>
       </c>
       <c r="E4">
-        <v>4.2688410000000001</v>
+        <v>5.3045410000000004</v>
       </c>
       <c r="F4">
-        <v>4.0400410000000004</v>
+        <v>5.0774239999999997</v>
       </c>
       <c r="G4">
-        <v>4.0830310000000001</v>
+        <v>4.4425350000000003</v>
       </c>
       <c r="H4">
-        <v>4.6600169999999999</v>
+        <v>7.459784</v>
       </c>
       <c r="I4">
-        <v>4.2676239999999996</v>
+        <v>5.3697869999999996</v>
       </c>
       <c r="J4">
-        <v>4.2576479999999997</v>
+        <v>5.3181510000000003</v>
       </c>
       <c r="K4">
-        <v>4.2768189999999997</v>
+        <v>5.5005480000000002</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2019</v>
+        <v>2023</v>
       </c>
       <c r="B5">
-        <v>4.7086980000000001</v>
+        <v>3.0087133844693503</v>
       </c>
       <c r="C5">
-        <v>4.696955</v>
+        <v>3.159149053692818</v>
       </c>
       <c r="D5">
-        <v>4.7087389999999996</v>
+        <v>5.7287340000000002</v>
       </c>
       <c r="E5">
-        <v>4.7143750000000004</v>
+        <v>5.5403929999999999</v>
       </c>
       <c r="F5">
-        <v>4.4233409999999997</v>
+        <v>5.2555430000000003</v>
       </c>
       <c r="G5">
-        <v>4.4047349999999996</v>
+        <v>4.5235349999999999</v>
       </c>
       <c r="H5">
-        <v>5.5792339999999996</v>
+        <v>8.0523349999999994</v>
       </c>
       <c r="I5">
-        <v>4.7614210000000003</v>
+        <v>5.6207760000000002</v>
       </c>
       <c r="J5">
-        <v>4.7161689999999998</v>
+        <v>5.5538780000000001</v>
       </c>
       <c r="K5">
-        <v>4.7309130000000001</v>
+        <v>5.7789529999999996</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2020</v>
+        <v>2024</v>
       </c>
       <c r="B6">
-        <v>5.1052530000000003</v>
+        <v>3.0236150225003562</v>
       </c>
       <c r="C6">
-        <v>5.0966829999999996</v>
+        <v>3.174795773625374</v>
       </c>
       <c r="D6">
-        <v>5.1183149999999999</v>
+        <v>6.0892749999999998</v>
       </c>
       <c r="E6">
-        <v>5.1889880000000002</v>
+        <v>5.8711599999999997</v>
       </c>
       <c r="F6">
-        <v>4.8038080000000001</v>
+        <v>5.4457409999999999</v>
       </c>
       <c r="G6">
-        <v>4.6971639999999999</v>
+        <v>4.6552749999999996</v>
       </c>
       <c r="H6">
-        <v>6.6139939999999999</v>
+        <v>8.6075890000000008</v>
       </c>
       <c r="I6">
-        <v>5.1673260000000001</v>
+        <v>5.8824370000000004</v>
       </c>
       <c r="J6">
-        <v>5.1110220000000002</v>
+        <v>5.8621939999999997</v>
       </c>
       <c r="K6">
-        <v>5.1855979999999997</v>
+        <v>6.0990859999999998</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="B7">
-        <v>5.1902160000000004</v>
+        <v>3.1512289841969809</v>
       </c>
       <c r="C7">
-        <v>5.1638599999999997</v>
+        <v>3.3087904334068301</v>
       </c>
       <c r="D7">
-        <v>5.2508660000000003</v>
+        <v>6.432633</v>
       </c>
       <c r="E7">
-        <v>5.2204249999999996</v>
+        <v>6.2562980000000001</v>
       </c>
       <c r="F7">
-        <v>4.9484219999999999</v>
+        <v>5.6475929999999996</v>
       </c>
       <c r="G7">
-        <v>4.5277120000000002</v>
+        <v>4.8336819999999996</v>
       </c>
       <c r="H7">
-        <v>7.0335140000000003</v>
+        <v>9.1337729999999997</v>
       </c>
       <c r="I7">
-        <v>5.2257680000000004</v>
+        <v>6.1611050000000001</v>
       </c>
       <c r="J7">
-        <v>5.1857009999999999</v>
+        <v>6.1274499999999996</v>
       </c>
       <c r="K7">
-        <v>5.3002320000000003</v>
+        <v>6.4655800000000001</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2022</v>
+        <v>2026</v>
       </c>
       <c r="B8">
-        <v>5.3517749999999999</v>
+        <v>3.2872336308161416</v>
       </c>
       <c r="C8">
-        <v>5.2909259999999998</v>
+        <v>3.4515953123569489</v>
       </c>
       <c r="D8">
-        <v>5.4649460000000003</v>
+        <v>6.7804270000000004</v>
       </c>
       <c r="E8">
-        <v>5.3045410000000004</v>
+        <v>6.6273280000000003</v>
       </c>
       <c r="F8">
-        <v>5.0774239999999997</v>
+        <v>5.8282299999999996</v>
       </c>
       <c r="G8">
-        <v>4.4425350000000003</v>
+        <v>5.0544000000000002</v>
       </c>
       <c r="H8">
-        <v>7.459784</v>
+        <v>9.53782</v>
       </c>
       <c r="I8">
-        <v>5.3697869999999996</v>
+        <v>6.417656</v>
       </c>
       <c r="J8">
-        <v>5.3181510000000003</v>
+        <v>6.3351199999999999</v>
       </c>
       <c r="K8">
-        <v>5.5005480000000002</v>
+        <v>6.8345479999999998</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2023</v>
+        <v>2027</v>
       </c>
       <c r="B9">
-        <v>5.6359969999999997</v>
+        <v>3.4097174803415933</v>
       </c>
       <c r="C9">
-        <v>5.5278409999999996</v>
+        <v>3.5802033543586731</v>
       </c>
       <c r="D9">
-        <v>5.7287340000000002</v>
+        <v>7.1353499999999999</v>
       </c>
       <c r="E9">
-        <v>5.5403929999999999</v>
+        <v>7.0558969999999999</v>
       </c>
       <c r="F9">
-        <v>5.2555430000000003</v>
+        <v>5.9496149999999997</v>
       </c>
       <c r="G9">
-        <v>4.5235349999999999</v>
+        <v>5.2546099999999996</v>
       </c>
       <c r="H9">
-        <v>8.0523349999999994</v>
+        <v>9.8988390000000006</v>
       </c>
       <c r="I9">
-        <v>5.6207760000000002</v>
+        <v>6.6698829999999996</v>
       </c>
       <c r="J9">
-        <v>5.5538780000000001</v>
+        <v>6.5501149999999999</v>
       </c>
       <c r="K9">
-        <v>5.7789529999999996</v>
+        <v>7.1753520000000002</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2024</v>
+        <v>2028</v>
       </c>
       <c r="B10">
-        <v>5.8818929999999998</v>
+        <v>3.4740086992581687</v>
       </c>
       <c r="C10">
-        <v>5.8011049999999997</v>
+        <v>3.6477091342210772</v>
       </c>
       <c r="D10">
-        <v>6.0892749999999998</v>
+        <v>7.3969610000000001</v>
       </c>
       <c r="E10">
-        <v>5.8711599999999997</v>
+        <v>7.4452230000000004</v>
       </c>
       <c r="F10">
-        <v>5.4457409999999999</v>
+        <v>6.1000170000000002</v>
       </c>
       <c r="G10">
-        <v>4.6552749999999996</v>
+        <v>5.411232</v>
       </c>
       <c r="H10">
-        <v>8.6075890000000008</v>
+        <v>10.238789000000001</v>
       </c>
       <c r="I10">
-        <v>5.8824370000000004</v>
+        <v>6.8608890000000002</v>
       </c>
       <c r="J10">
-        <v>5.8621939999999997</v>
+        <v>6.8136260000000002</v>
       </c>
       <c r="K10">
-        <v>6.0990859999999998</v>
+        <v>7.5210530000000002</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2025</v>
+        <v>2029</v>
       </c>
       <c r="B11">
-        <v>6.1772770000000001</v>
+        <v>3.7310661673545837</v>
       </c>
       <c r="C11">
-        <v>6.0548599999999997</v>
+        <v>3.9176194757223133</v>
       </c>
       <c r="D11">
-        <v>6.432633</v>
+        <v>7.7163729999999999</v>
       </c>
       <c r="E11">
-        <v>6.2562980000000001</v>
+        <v>7.7466499999999998</v>
       </c>
       <c r="F11">
-        <v>5.6475929999999996</v>
+        <v>6.2988280000000003</v>
       </c>
       <c r="G11">
-        <v>4.8336819999999996</v>
+        <v>5.5285399999999996</v>
       </c>
       <c r="H11">
-        <v>9.1337729999999997</v>
+        <v>10.625026</v>
       </c>
       <c r="I11">
-        <v>6.1611050000000001</v>
+        <v>7.1541930000000002</v>
       </c>
       <c r="J11">
-        <v>6.1274499999999996</v>
+        <v>7.0545530000000003</v>
       </c>
       <c r="K11">
-        <v>6.4655800000000001</v>
+        <v>7.8445650000000002</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2026</v>
+        <v>2030</v>
       </c>
       <c r="B12">
-        <v>6.3641059999999996</v>
+        <v>3.932691752910614</v>
       </c>
       <c r="C12">
-        <v>6.2555209999999999</v>
+        <v>4.1293263405561449</v>
       </c>
       <c r="D12">
-        <v>6.7804270000000004</v>
+        <v>8.0604099999999992</v>
       </c>
       <c r="E12">
-        <v>6.6273280000000003</v>
+        <v>8.0435619999999997</v>
       </c>
       <c r="F12">
-        <v>5.8282299999999996</v>
+        <v>6.4277740000000003</v>
       </c>
       <c r="G12">
-        <v>5.0544000000000002</v>
+        <v>5.6155119999999998</v>
       </c>
       <c r="H12">
-        <v>9.53782</v>
+        <v>10.795173999999999</v>
       </c>
       <c r="I12">
-        <v>6.417656</v>
+        <v>7.3648360000000004</v>
       </c>
       <c r="J12">
-        <v>6.3351199999999999</v>
+        <v>7.3219260000000004</v>
       </c>
       <c r="K12">
-        <v>6.8345479999999998</v>
+        <v>8.254365</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2027</v>
+        <v>2031</v>
       </c>
       <c r="B13">
-        <v>6.566014</v>
+        <v>4.0979781548182173</v>
       </c>
       <c r="C13">
-        <v>6.428801</v>
+        <v>4.3028770625591282</v>
       </c>
       <c r="D13">
-        <v>7.1353499999999999</v>
+        <v>8.3579670000000004</v>
       </c>
       <c r="E13">
-        <v>7.0558969999999999</v>
+        <v>8.4530119999999993</v>
       </c>
       <c r="F13">
-        <v>5.9496149999999997</v>
+        <v>6.582757</v>
       </c>
       <c r="G13">
-        <v>5.2546099999999996</v>
+        <v>5.7347219999999997</v>
       </c>
       <c r="H13">
-        <v>9.8988390000000006</v>
+        <v>11.030429</v>
       </c>
       <c r="I13">
-        <v>6.6698829999999996</v>
+        <v>7.496435</v>
       </c>
       <c r="J13">
-        <v>6.5501149999999999</v>
+        <v>7.4886100000000004</v>
       </c>
       <c r="K13">
-        <v>7.1753520000000002</v>
+        <v>8.5158550000000002</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2028</v>
+        <v>2032</v>
       </c>
       <c r="B14">
-        <v>6.7123970000000002</v>
+        <v>4.1916568676630659</v>
       </c>
       <c r="C14">
-        <v>6.6402929999999998</v>
+        <v>4.4012397110462196</v>
       </c>
       <c r="D14">
-        <v>7.3969610000000001</v>
+        <v>8.6945230000000002</v>
       </c>
       <c r="E14">
-        <v>7.4452230000000004</v>
+        <v>8.8341539999999998</v>
       </c>
       <c r="F14">
-        <v>6.1000170000000002</v>
+        <v>6.7415929999999999</v>
       </c>
       <c r="G14">
-        <v>5.411232</v>
+        <v>5.8344370000000003</v>
       </c>
       <c r="H14">
-        <v>10.238789000000001</v>
+        <v>11.327975</v>
       </c>
       <c r="I14">
-        <v>6.8608890000000002</v>
+        <v>7.5974139999999997</v>
       </c>
       <c r="J14">
-        <v>6.8136260000000002</v>
+        <v>7.6356789999999997</v>
       </c>
       <c r="K14">
-        <v>7.5210530000000002</v>
+        <v>8.8024679999999993</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2029</v>
+        <v>2033</v>
       </c>
       <c r="B15">
-        <v>6.9405780000000004</v>
+        <v>4.4818841616312666</v>
       </c>
       <c r="C15">
-        <v>6.8538639999999997</v>
+        <v>4.7059783697128301</v>
       </c>
       <c r="D15">
-        <v>7.7163729999999999</v>
+        <v>9.0464300000000009</v>
       </c>
       <c r="E15">
-        <v>7.7466499999999998</v>
+        <v>9.2315459999999998</v>
       </c>
       <c r="F15">
-        <v>6.2988280000000003</v>
+        <v>6.9201550000000003</v>
       </c>
       <c r="G15">
-        <v>5.5285399999999996</v>
+        <v>5.9085099999999997</v>
       </c>
       <c r="H15">
-        <v>10.625026</v>
+        <v>11.608306000000001</v>
       </c>
       <c r="I15">
-        <v>7.1541930000000002</v>
+        <v>7.7223990000000002</v>
       </c>
       <c r="J15">
-        <v>7.0545530000000003</v>
+        <v>7.7712450000000004</v>
       </c>
       <c r="K15">
-        <v>7.8445650000000002</v>
+        <v>9.1069569999999995</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2030</v>
+        <v>2034</v>
       </c>
       <c r="B16">
-        <v>7.085915</v>
+        <v>4.7039756377538042</v>
       </c>
       <c r="C16">
-        <v>7.0670190000000002</v>
+        <v>4.9391744196414944</v>
       </c>
       <c r="D16">
-        <v>8.0604099999999992</v>
+        <v>9.3883229999999998</v>
       </c>
       <c r="E16">
-        <v>8.0435619999999997</v>
+        <v>9.6809740000000009</v>
       </c>
       <c r="F16">
-        <v>6.4277740000000003</v>
+        <v>7.0971399999999996</v>
       </c>
       <c r="G16">
-        <v>5.6155119999999998</v>
+        <v>6.0016540000000003</v>
       </c>
       <c r="H16">
-        <v>10.795173999999999</v>
+        <v>12.035529</v>
       </c>
       <c r="I16">
-        <v>7.3648360000000004</v>
+        <v>7.9324719999999997</v>
       </c>
       <c r="J16">
-        <v>7.3219260000000004</v>
+        <v>7.9283140000000003</v>
       </c>
       <c r="K16">
-        <v>8.254365</v>
+        <v>9.4188550000000006</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2031</v>
+        <v>2035</v>
       </c>
       <c r="B17">
-        <v>7.2424580000000001</v>
+        <v>4.9315100113550825</v>
       </c>
       <c r="C17">
-        <v>7.27156</v>
+        <v>5.1780855119228368</v>
       </c>
       <c r="D17">
-        <v>8.3579670000000004</v>
+        <v>9.7302269999999993</v>
       </c>
       <c r="E17">
-        <v>8.4530119999999993</v>
+        <v>10.049029000000001</v>
       </c>
       <c r="F17">
-        <v>6.582757</v>
+        <v>7.2470509999999999</v>
       </c>
       <c r="G17">
-        <v>5.7347219999999997</v>
+        <v>6.1221389999999998</v>
       </c>
       <c r="H17">
-        <v>11.030429</v>
+        <v>12.432501999999999</v>
       </c>
       <c r="I17">
-        <v>7.496435</v>
+        <v>8.1331500000000005</v>
       </c>
       <c r="J17">
-        <v>7.4886100000000004</v>
+        <v>8.1163039999999995</v>
       </c>
       <c r="K17">
-        <v>8.5158550000000002</v>
+        <v>9.7423509999999993</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2032</v>
+        <v>2036</v>
       </c>
       <c r="B18">
-        <v>7.417484</v>
+        <v>5.142708420753479</v>
       </c>
       <c r="C18">
-        <v>7.4929079999999999</v>
+        <v>5.399843841791153</v>
       </c>
       <c r="D18">
-        <v>8.6945230000000002</v>
+        <v>10.253242</v>
       </c>
       <c r="E18">
-        <v>8.8341539999999998</v>
+        <v>10.467165</v>
       </c>
       <c r="F18">
-        <v>6.7415929999999999</v>
+        <v>7.5113750000000001</v>
       </c>
       <c r="G18">
-        <v>5.8344370000000003</v>
+        <v>6.28207</v>
       </c>
       <c r="H18">
-        <v>11.327975</v>
+        <v>12.973235000000001</v>
       </c>
       <c r="I18">
-        <v>7.5974139999999997</v>
+        <v>8.4020399999999995</v>
       </c>
       <c r="J18">
-        <v>7.6356789999999997</v>
+        <v>8.4497309999999999</v>
       </c>
       <c r="K18">
-        <v>8.8024679999999993</v>
+        <v>10.205553999999999</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2033</v>
+        <v>2037</v>
       </c>
       <c r="B19">
-        <v>7.5779769999999997</v>
+        <v>5.2559186220169067</v>
       </c>
       <c r="C19">
-        <v>7.6944140000000001</v>
+        <v>5.5187145531177526</v>
       </c>
       <c r="D19">
-        <v>9.0464300000000009</v>
+        <v>10.680801000000001</v>
       </c>
       <c r="E19">
-        <v>9.2315459999999998</v>
+        <v>10.782007999999999</v>
       </c>
       <c r="F19">
-        <v>6.9201550000000003</v>
+        <v>7.7217399999999996</v>
       </c>
       <c r="G19">
-        <v>5.9085099999999997</v>
+        <v>6.398015</v>
       </c>
       <c r="H19">
-        <v>11.608306000000001</v>
+        <v>13.393464</v>
       </c>
       <c r="I19">
-        <v>7.7223990000000002</v>
+        <v>8.5654979999999998</v>
       </c>
       <c r="J19">
-        <v>7.7712450000000004</v>
+        <v>8.7629889999999993</v>
       </c>
       <c r="K19">
-        <v>9.1069569999999995</v>
+        <v>10.640934</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2034</v>
+        <v>2038</v>
       </c>
       <c r="B20">
-        <v>7.7584619999999997</v>
+        <v>5.3300158580144243</v>
       </c>
       <c r="C20">
-        <v>7.9154059999999999</v>
+        <v>5.5965166509151461</v>
       </c>
       <c r="D20">
-        <v>9.3883229999999998</v>
+        <v>11.153608999999999</v>
       </c>
       <c r="E20">
-        <v>9.6809740000000009</v>
+        <v>11.183285</v>
       </c>
       <c r="F20">
-        <v>7.0971399999999996</v>
+        <v>7.9785769999999996</v>
       </c>
       <c r="G20">
-        <v>6.0016540000000003</v>
+        <v>6.5716150000000004</v>
       </c>
       <c r="H20">
-        <v>12.035529</v>
+        <v>13.854094999999999</v>
       </c>
       <c r="I20">
-        <v>7.9324719999999997</v>
+        <v>8.8772570000000002</v>
       </c>
       <c r="J20">
-        <v>7.9283140000000003</v>
+        <v>9.1231729999999995</v>
       </c>
       <c r="K20">
-        <v>9.4188550000000006</v>
+        <v>11.222917000000001</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2035</v>
+        <v>2039</v>
       </c>
       <c r="B21">
-        <v>7.926984</v>
+        <v>5.4953441619873047</v>
       </c>
       <c r="C21">
-        <v>8.1695890000000002</v>
+        <v>5.7701113700866697</v>
       </c>
       <c r="D21">
-        <v>9.7302269999999993</v>
+        <v>11.637653999999999</v>
       </c>
       <c r="E21">
-        <v>10.049029000000001</v>
+        <v>11.793828</v>
       </c>
       <c r="F21">
-        <v>7.2470509999999999</v>
+        <v>8.1683240000000001</v>
       </c>
       <c r="G21">
-        <v>6.1221389999999998</v>
+        <v>6.7884190000000002</v>
       </c>
       <c r="H21">
-        <v>12.432501999999999</v>
+        <v>14.281375000000001</v>
       </c>
       <c r="I21">
-        <v>8.1331500000000005</v>
+        <v>9.1816530000000007</v>
       </c>
       <c r="J21">
-        <v>8.1163039999999995</v>
+        <v>9.346292</v>
       </c>
       <c r="K21">
-        <v>9.7423509999999993</v>
+        <v>11.71035</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2036</v>
+        <v>2040</v>
       </c>
       <c r="B22">
-        <v>8.2570969999999999</v>
+        <v>5.6733103195826216</v>
       </c>
       <c r="C22">
-        <v>8.4741289999999996</v>
+        <v>5.956975835561753</v>
       </c>
       <c r="D22">
-        <v>10.253242</v>
+        <v>12.102088999999999</v>
       </c>
       <c r="E22">
-        <v>10.467165</v>
+        <v>11.886378000000001</v>
       </c>
       <c r="F22">
-        <v>7.5113750000000001</v>
+        <v>8.4208669999999994</v>
       </c>
       <c r="G22">
-        <v>6.28207</v>
+        <v>6.9530770000000004</v>
       </c>
       <c r="H22">
-        <v>12.973235000000001</v>
+        <v>14.720748</v>
       </c>
       <c r="I22">
-        <v>8.4020399999999995</v>
+        <v>9.4102180000000004</v>
       </c>
       <c r="J22">
-        <v>8.4497309999999999</v>
+        <v>9.5872240000000009</v>
       </c>
       <c r="K22">
-        <v>10.205553999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2037</v>
-      </c>
-      <c r="B23">
-        <v>8.4714019999999994</v>
-      </c>
-      <c r="C23">
-        <v>8.7403469999999999</v>
-      </c>
-      <c r="D23">
-        <v>10.680801000000001</v>
-      </c>
-      <c r="E23">
-        <v>10.782007999999999</v>
-      </c>
-      <c r="F23">
-        <v>7.7217399999999996</v>
-      </c>
-      <c r="G23">
-        <v>6.398015</v>
-      </c>
-      <c r="H23">
-        <v>13.393464</v>
-      </c>
-      <c r="I23">
-        <v>8.5654979999999998</v>
-      </c>
-      <c r="J23">
-        <v>8.7629889999999993</v>
-      </c>
-      <c r="K23">
-        <v>10.640934</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2038</v>
-      </c>
-      <c r="B24">
-        <v>8.7667529999999996</v>
-      </c>
-      <c r="C24">
-        <v>9.0837990000000008</v>
-      </c>
-      <c r="D24">
-        <v>11.153608999999999</v>
-      </c>
-      <c r="E24">
-        <v>11.183285</v>
-      </c>
-      <c r="F24">
-        <v>7.9785769999999996</v>
-      </c>
-      <c r="G24">
-        <v>6.5716150000000004</v>
-      </c>
-      <c r="H24">
-        <v>13.854094999999999</v>
-      </c>
-      <c r="I24">
-        <v>8.8772570000000002</v>
-      </c>
-      <c r="J24">
-        <v>9.1231729999999995</v>
-      </c>
-      <c r="K24">
-        <v>11.222917000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2039</v>
-      </c>
-      <c r="B25">
-        <v>9.0416290000000004</v>
-      </c>
-      <c r="C25">
-        <v>9.3653519999999997</v>
-      </c>
-      <c r="D25">
-        <v>11.637653999999999</v>
-      </c>
-      <c r="E25">
-        <v>11.793828</v>
-      </c>
-      <c r="F25">
-        <v>8.1683240000000001</v>
-      </c>
-      <c r="G25">
-        <v>6.7884190000000002</v>
-      </c>
-      <c r="H25">
-        <v>14.281375000000001</v>
-      </c>
-      <c r="I25">
-        <v>9.1816530000000007</v>
-      </c>
-      <c r="J25">
-        <v>9.346292</v>
-      </c>
-      <c r="K25">
-        <v>11.71035</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2040</v>
-      </c>
-      <c r="B26">
-        <v>9.2946580000000001</v>
-      </c>
-      <c r="C26">
-        <v>9.6309780000000007</v>
-      </c>
-      <c r="D26">
-        <v>12.102088999999999</v>
-      </c>
-      <c r="E26">
-        <v>11.886378000000001</v>
-      </c>
-      <c r="F26">
-        <v>8.4208669999999994</v>
-      </c>
-      <c r="G26">
-        <v>6.9530770000000004</v>
-      </c>
-      <c r="H26">
-        <v>14.720748</v>
-      </c>
-      <c r="I26">
-        <v>9.4102180000000004</v>
-      </c>
-      <c r="J26">
-        <v>9.5872240000000009</v>
-      </c>
-      <c r="K26">
         <v>12.167077000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2041</v>
-      </c>
-      <c r="B27">
-        <v>9.5743650000000002</v>
-      </c>
-      <c r="C27">
-        <v>9.9301960000000005</v>
-      </c>
-      <c r="D27">
-        <v>12.577082000000001</v>
-      </c>
-      <c r="E27">
-        <v>12.543870999999999</v>
-      </c>
-      <c r="F27">
-        <v>8.7032089999999993</v>
-      </c>
-      <c r="G27">
-        <v>7.1036710000000003</v>
-      </c>
-      <c r="H27">
-        <v>15.222104</v>
-      </c>
-      <c r="I27">
-        <v>9.672288</v>
-      </c>
-      <c r="J27">
-        <v>9.9033259999999999</v>
-      </c>
-      <c r="K27">
-        <v>12.698748999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>2042</v>
-      </c>
-      <c r="B28">
-        <v>9.9134220000000006</v>
-      </c>
-      <c r="C28">
-        <v>10.271685</v>
-      </c>
-      <c r="D28">
-        <v>13.096859</v>
-      </c>
-      <c r="E28">
-        <v>12.698318</v>
-      </c>
-      <c r="F28">
-        <v>8.9984260000000003</v>
-      </c>
-      <c r="G28">
-        <v>7.2652599999999996</v>
-      </c>
-      <c r="H28">
-        <v>15.619415999999999</v>
-      </c>
-      <c r="I28">
-        <v>9.9782460000000004</v>
-      </c>
-      <c r="J28">
-        <v>10.292391</v>
-      </c>
-      <c r="K28">
-        <v>13.21564</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>2043</v>
-      </c>
-      <c r="B29">
-        <v>10.222052</v>
-      </c>
-      <c r="C29">
-        <v>10.568159</v>
-      </c>
-      <c r="D29">
-        <v>13.646774000000001</v>
-      </c>
-      <c r="E29">
-        <v>13.347929000000001</v>
-      </c>
-      <c r="F29">
-        <v>9.2801930000000006</v>
-      </c>
-      <c r="G29">
-        <v>7.4497900000000001</v>
-      </c>
-      <c r="H29">
-        <v>16.137173000000001</v>
-      </c>
-      <c r="I29">
-        <v>10.313761</v>
-      </c>
-      <c r="J29">
-        <v>10.628504</v>
-      </c>
-      <c r="K29">
-        <v>13.758086</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>2044</v>
-      </c>
-      <c r="B30">
-        <v>10.564087000000001</v>
-      </c>
-      <c r="C30">
-        <v>10.928451000000001</v>
-      </c>
-      <c r="D30">
-        <v>14.312735999999999</v>
-      </c>
-      <c r="E30">
-        <v>13.923943</v>
-      </c>
-      <c r="F30">
-        <v>9.6485099999999999</v>
-      </c>
-      <c r="G30">
-        <v>7.6720889999999997</v>
-      </c>
-      <c r="H30">
-        <v>17.059322000000002</v>
-      </c>
-      <c r="I30">
-        <v>10.689742000000001</v>
-      </c>
-      <c r="J30">
-        <v>11.047209000000001</v>
-      </c>
-      <c r="K30">
-        <v>14.401305000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>2045</v>
-      </c>
-      <c r="B31">
-        <v>10.921581</v>
-      </c>
-      <c r="C31">
-        <v>11.354794999999999</v>
-      </c>
-      <c r="D31">
-        <v>15.013617999999999</v>
-      </c>
-      <c r="E31">
-        <v>14.423067</v>
-      </c>
-      <c r="F31">
-        <v>10.000031999999999</v>
-      </c>
-      <c r="G31">
-        <v>7.8512709999999997</v>
-      </c>
-      <c r="H31">
-        <v>17.948364000000002</v>
-      </c>
-      <c r="I31">
-        <v>11.081963999999999</v>
-      </c>
-      <c r="J31">
-        <v>11.534409999999999</v>
-      </c>
-      <c r="K31">
-        <v>15.103513</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>2046</v>
-      </c>
-      <c r="B32">
-        <v>11.289496</v>
-      </c>
-      <c r="C32">
-        <v>11.597038</v>
-      </c>
-      <c r="D32">
-        <v>15.724034</v>
-      </c>
-      <c r="E32">
-        <v>14.888631</v>
-      </c>
-      <c r="F32">
-        <v>10.334372999999999</v>
-      </c>
-      <c r="G32">
-        <v>8.0700950000000002</v>
-      </c>
-      <c r="H32">
-        <v>18.688831</v>
-      </c>
-      <c r="I32">
-        <v>11.498405</v>
-      </c>
-      <c r="J32">
-        <v>11.951684999999999</v>
-      </c>
-      <c r="K32">
-        <v>15.778893</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>2047</v>
-      </c>
-      <c r="B33">
-        <v>11.673401</v>
-      </c>
-      <c r="C33">
-        <v>12.189022</v>
-      </c>
-      <c r="D33">
-        <v>16.431069999999998</v>
-      </c>
-      <c r="E33">
-        <v>15.360474999999999</v>
-      </c>
-      <c r="F33">
-        <v>10.71984</v>
-      </c>
-      <c r="G33">
-        <v>8.3279829999999997</v>
-      </c>
-      <c r="H33">
-        <v>19.598654</v>
-      </c>
-      <c r="I33">
-        <v>11.926309</v>
-      </c>
-      <c r="J33">
-        <v>12.391546</v>
-      </c>
-      <c r="K33">
-        <v>16.436577</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>2048</v>
-      </c>
-      <c r="B34">
-        <v>12.140743000000001</v>
-      </c>
-      <c r="C34">
-        <v>12.824095</v>
-      </c>
-      <c r="D34">
-        <v>17.188110000000002</v>
-      </c>
-      <c r="E34">
-        <v>15.910882000000001</v>
-      </c>
-      <c r="F34">
-        <v>11.131232000000001</v>
-      </c>
-      <c r="G34">
-        <v>8.5844070000000006</v>
-      </c>
-      <c r="H34">
-        <v>20.442764</v>
-      </c>
-      <c r="I34">
-        <v>12.364013</v>
-      </c>
-      <c r="J34">
-        <v>12.888714999999999</v>
-      </c>
-      <c r="K34">
-        <v>17.124769000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>2049</v>
-      </c>
-      <c r="B35">
-        <v>12.592207999999999</v>
-      </c>
-      <c r="C35">
-        <v>13.243323999999999</v>
-      </c>
-      <c r="D35">
-        <v>17.977461000000002</v>
-      </c>
-      <c r="E35">
-        <v>16.415749000000002</v>
-      </c>
-      <c r="F35">
-        <v>11.505298</v>
-      </c>
-      <c r="G35">
-        <v>8.8621130000000008</v>
-      </c>
-      <c r="H35">
-        <v>21.592495</v>
-      </c>
-      <c r="I35">
-        <v>12.810791</v>
-      </c>
-      <c r="J35">
-        <v>13.251673</v>
-      </c>
-      <c r="K35">
-        <v>18.048248000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>2050</v>
-      </c>
-      <c r="B36">
-        <v>13.098245</v>
-      </c>
-      <c r="C36">
-        <v>13.752340999999999</v>
-      </c>
-      <c r="D36">
-        <v>18.939449</v>
-      </c>
-      <c r="E36">
-        <v>16.978166999999999</v>
-      </c>
-      <c r="F36">
-        <v>11.957445</v>
-      </c>
-      <c r="G36">
-        <v>9.1261310000000009</v>
-      </c>
-      <c r="H36">
-        <v>22.767537999999998</v>
-      </c>
-      <c r="I36">
-        <v>13.33146</v>
-      </c>
-      <c r="J36">
-        <v>13.777882999999999</v>
-      </c>
-      <c r="K36">
-        <v>19.089328999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>